<commit_message>
code, notes, util updated
</commit_message>
<xml_diff>
--- a/eosio_vs_eth.xlsx
+++ b/eosio_vs_eth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Coding\github_repos\ethio_playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38123D75-A132-45AD-BFB2-174620F8E992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6067C266-5E33-419D-A8F2-C6F658806187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{525611D5-18D7-41F8-A371-26E5FA616275}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>EOSIO</t>
   </si>
@@ -119,9 +119,6 @@
     <t>64 bit</t>
   </si>
   <si>
-    <t>20 bytes</t>
-  </si>
-  <si>
     <t>uint32_t</t>
   </si>
   <si>
@@ -129,6 +126,44 @@
   </si>
   <si>
     <t>32 bit</t>
+  </si>
+  <si>
+    <t>msg.value</t>
+  </si>
+  <si>
+    <t>qty.amount</t>
+  </si>
+  <si>
+    <t>token quantity amount</t>
+  </si>
+  <si>
+    <t>type: uint64_t
+asset is class where amount is the actual value</t>
+  </si>
+  <si>
+    <t>type: uint (wei)
+NOTE: uint is alias for uint256</t>
+  </si>
+  <si>
+    <t>Constructor</t>
+  </si>
+  <si>
+    <t>others\eosio_vs_eth_constructor.png</t>
+  </si>
+  <si>
+    <t>20 bytes = 160 bits</t>
+  </si>
+  <si>
+    <t>used in token quantity balance, deposit, withdraw, transfer</t>
+  </si>
+  <si>
+    <t>to initialize</t>
+  </si>
+  <si>
+    <t>account name, filename, contract name must match</t>
+  </si>
+  <si>
+    <t>filename, contract name must match</t>
   </si>
 </sst>
 </file>
@@ -201,7 +236,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -226,6 +261,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -544,18 +582,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E29F14-69FA-4A1C-8576-9B2A132A653B}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="43" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.21875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.5546875" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.6640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5546875" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
@@ -579,7 +617,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -596,7 +634,7 @@
         <v>29</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
@@ -671,33 +709,57 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+    <row r="8" spans="1:6" ht="50.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
@@ -758,8 +820,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{097BD82B-43D0-478B-A616-A3D0ED0E8BD4}"/>
+    <hyperlink ref="B9" r:id="rId2" xr:uid="{BC7E8774-8200-4B94-B8CC-23F9BC4821B0}"/>
+    <hyperlink ref="C9" r:id="rId3" xr:uid="{62F04013-DE01-4572-A1DD-4EEF9F2C8F72}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
gas optimization notes added, token precision vs decimal added
</commit_message>
<xml_diff>
--- a/eosio_vs_eth.xlsx
+++ b/eosio_vs_eth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Coding\github_repos\ethio_playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0A2D29-D5B4-49D8-B549-8671E06CE931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DD6868-16B2-49F3-9500-623B901C3FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{525611D5-18D7-41F8-A371-26E5FA616275}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t>EOSIO</t>
   </si>
@@ -222,6 +222,21 @@
   </si>
   <si>
     <t>transfer()</t>
+  </si>
+  <si>
+    <t>name of decimals in a token amount</t>
+  </si>
+  <si>
+    <t>token precision (4 max.)</t>
+  </si>
+  <si>
+    <t>token decimals (18 max.)</t>
+  </si>
+  <si>
+    <t>lowest value, unit = 10^(-18), wei</t>
+  </si>
+  <si>
+    <t>lowest value, unit = 0.0001, -</t>
   </si>
 </sst>
 </file>
@@ -628,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E29F14-69FA-4A1C-8576-9B2A132A653B}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -885,13 +900,22 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+    <row r="15" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>

</xml_diff>

<commit_message>
token with decimal representation
</commit_message>
<xml_diff>
--- a/eosio_vs_eth.xlsx
+++ b/eosio_vs_eth.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Coding\github_repos\ethio_playground\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6E69A6-39E3-494D-97CA-8B865D297FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE49D4DB-568B-4E99-8B7E-89DEF5E1AC96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{525611D5-18D7-41F8-A371-26E5FA616275}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="107">
   <si>
     <t>EOSIO</t>
   </si>
@@ -422,6 +422,23 @@
   </si>
   <si>
     <t>account keys storage folder</t>
+  </si>
+  <si>
+    <t>Token with decimal representation</t>
+  </si>
+  <si>
+    <t>usage in contract code.
+NOTE: There is no way to represent decimal, so that's why this method is chosen.</t>
+  </si>
+  <si>
+    <t>9 EOSIO token is represented in code as 9*10^4
+Here, 4 is decimal.
+9.56 ~ 9.56*10^4</t>
+  </si>
+  <si>
+    <t>9 ERC20 token is represented in code as 9*10^18
+Here, 18 is decimal.
+9.56 ~ 9.56*10^18</t>
   </si>
 </sst>
 </file>
@@ -551,8 +568,8 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>198274</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="2" name="Ink 1">
@@ -571,7 +588,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="2" name="Ink 1">
@@ -930,10 +947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E29F14-69FA-4A1C-8576-9B2A132A653B}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
@@ -1294,7 +1311,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" ht="151.19999999999999" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="117.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>79</v>
       </c>
@@ -1329,6 +1346,22 @@
       <c r="F22" s="2" t="s">
         <v>81</v>
       </c>
+    </row>
+    <row r="23" spans="1:6" ht="84" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
added expect await, diff eosio vs eth interface
</commit_message>
<xml_diff>
--- a/eosio_vs_eth.xlsx
+++ b/eosio_vs_eth.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Coding\github_repos\ethio_playground\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhi3700/F/coding/github_repos/evm_playground/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE49D4DB-568B-4E99-8B7E-89DEF5E1AC96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C733ACC-B131-9143-8D78-268116CF1165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{525611D5-18D7-41F8-A371-26E5FA616275}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14440" xr2:uid="{525611D5-18D7-41F8-A371-26E5FA616275}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$23</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="113">
   <si>
     <t>EOSIO</t>
   </si>
@@ -439,6 +442,28 @@
     <t>9 ERC20 token is represented in code as 9*10^18
 Here, 18 is decimal.
 9.56 ~ 9.56*10^18</t>
+  </si>
+  <si>
+    <t>Interface</t>
+  </si>
+  <si>
+    <t>using distribute_action  = action_wrapper&lt;"distribute"_n, &amp;terraworlds::distribute&gt;;</t>
+  </si>
+  <si>
+    <t>interface InterfaceTerraworlds {
+   function distribute(uint256 nextId) external returns (bool);
+}</t>
+  </si>
+  <si>
+    <t>Using contract's function from inside another contract.</t>
+  </si>
+  <si>
+    <t>Write the function inside the contract &amp; make the function available to external contract(s) using action_wrapper</t>
+  </si>
+  <si>
+    <t>Write the function inside the contract &amp; make the function available via 2methods:
+M-1: writing interface module inside another contract or 
+M-2: creating a file with interface module inside.</t>
   </si>
 </sst>
 </file>
@@ -566,7 +591,7 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>349646</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>198274</xdr:rowOff>
+      <xdr:rowOff>196114</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
       <mc:Choice Requires="xdr14">
@@ -947,24 +972,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E29F14-69FA-4A1C-8576-9B2A132A653B}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="43" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.21875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="49.1640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="34.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="28.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="3"/>
+    <col min="6" max="6" width="28.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -984,7 +1009,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="409.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>86</v>
       </c>
@@ -1004,7 +1029,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="35.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>87</v>
       </c>
@@ -1022,7 +1047,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="67.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>72</v>
       </c>
@@ -1042,7 +1067,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>101</v>
       </c>
@@ -1056,7 +1081,7 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>102</v>
       </c>
@@ -1076,7 +1101,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1096,7 +1121,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1112,7 +1137,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -1130,7 +1155,7 @@
       </c>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1146,7 +1171,7 @@
       </c>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -1160,7 +1185,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" ht="50.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>28</v>
       </c>
@@ -1180,7 +1205,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>31</v>
       </c>
@@ -1200,7 +1225,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="50.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -1216,7 +1241,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
@@ -1236,7 +1261,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>49</v>
       </c>
@@ -1250,7 +1275,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>52</v>
       </c>
@@ -1264,7 +1289,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>55</v>
       </c>
@@ -1278,7 +1303,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>58</v>
       </c>
@@ -1295,7 +1320,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>65</v>
       </c>
@@ -1311,7 +1336,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" ht="117.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>79</v>
       </c>
@@ -1329,7 +1354,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="117.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="119" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>82</v>
       </c>
@@ -1347,7 +1372,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="84" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>103</v>
       </c>
@@ -1363,7 +1388,28 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
+    <row r="24" spans="1:6" ht="153" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:F23" xr:uid="{24E29F14-69FA-4A1C-8576-9B2A132A653B}"/>
   <hyperlinks>
     <hyperlink ref="E9" r:id="rId1" xr:uid="{097BD82B-43D0-478B-A616-A3D0ED0E8BD4}"/>
     <hyperlink ref="B13" r:id="rId2" xr:uid="{BC7E8774-8200-4B94-B8CC-23F9BC4821B0}"/>

</xml_diff>

<commit_message>
merkle tree link added, eosio vs eth diff modified
</commit_message>
<xml_diff>
--- a/eosio_vs_eth.xlsx
+++ b/eosio_vs_eth.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhi3700/F/coding/github_repos/evm_playground/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C733ACC-B131-9143-8D78-268116CF1165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBAED13E-8C21-E846-8278-4887A066968C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14440" xr2:uid="{525611D5-18D7-41F8-A371-26E5FA616275}"/>
   </bookViews>
@@ -22,6 +22,16 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -974,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E29F14-69FA-4A1C-8576-9B2A132A653B}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="135" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -989,7 +999,7 @@
     <col min="7" max="16384" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1261,7 +1271,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>49</v>
       </c>

</xml_diff>